<commit_message>
Modify Read excel file code, Added read CSV file class, Added date helpers
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -14,45 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>firstname</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>lastname</t>
+    <t>Testusername</t>
   </si>
   <si>
-    <t>postcode</t>
+    <t>Testpassword</t>
   </si>
   <si>
-    <t>TestFname1</t>
-  </si>
-  <si>
-    <t>TestLname1</t>
-  </si>
-  <si>
-    <t>TestFname2</t>
-  </si>
-  <si>
-    <t>TestFname3</t>
-  </si>
-  <si>
-    <t>TestFname4</t>
-  </si>
-  <si>
-    <t>TestFname5</t>
-  </si>
-  <si>
-    <t>TestLname2</t>
-  </si>
-  <si>
-    <t>TestLname3</t>
-  </si>
-  <si>
-    <t>TestLname4</t>
-  </si>
-  <si>
-    <t>TestLname5</t>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -394,78 +367,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>60020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>60021</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>60022</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>60023</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>60024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>